<commit_message>
subi cambios anahi puedes ver este log
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/TMME.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/TMME.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="648"/>
   </bookViews>
   <sheets>
     <sheet name="NOMINA" sheetId="38" r:id="rId1"/>
@@ -5923,11 +5923,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:DU5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="CC5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="6" ySplit="4" topLeftCell="V5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AI17" sqref="AI17"/>
+      <selection pane="bottomRight" activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5944,13 +5944,20 @@
     <col min="12" max="12" width="19.85546875" customWidth="1"/>
     <col min="13" max="13" width="28.7109375" customWidth="1"/>
     <col min="14" max="14" width="15.140625" customWidth="1"/>
-    <col min="71" max="71" width="15.42578125" customWidth="1"/>
+    <col min="24" max="24" width="12.85546875" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" customWidth="1"/>
+    <col min="30" max="30" width="15.140625" customWidth="1"/>
+    <col min="37" max="37" width="14.42578125" customWidth="1"/>
+    <col min="40" max="43" width="14.42578125" customWidth="1"/>
+    <col min="71" max="71" width="19" customWidth="1"/>
+    <col min="72" max="72" width="17.7109375" customWidth="1"/>
     <col min="81" max="81" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="14.85546875" customWidth="1"/>
-    <col min="85" max="85" width="15.7109375" customWidth="1"/>
+    <col min="84" max="84" width="15.85546875" customWidth="1"/>
+    <col min="85" max="85" width="19.140625" customWidth="1"/>
     <col min="91" max="91" width="14" customWidth="1"/>
-    <col min="92" max="92" width="13.7109375" customWidth="1"/>
-    <col min="93" max="93" width="15.7109375" customWidth="1"/>
+    <col min="92" max="92" width="16.28515625" customWidth="1"/>
+    <col min="93" max="93" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:125" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6682,7 +6689,7 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="B3:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="110" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="110" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sin recuperar aun x3
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/TMME.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/TMME.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NOMINA" sheetId="38" r:id="rId1"/>
@@ -5923,7 +5923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:DU5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="4" topLeftCell="V5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -6689,8 +6689,8 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="B3:P56"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>